<commit_message>
More classifiers and better code for running test data
</commit_message>
<xml_diff>
--- a/sentiment-classifier/sandbox/resources/sample-testdata.xlsx
+++ b/sentiment-classifier/sandbox/resources/sample-testdata.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="240" windowWidth="8580" windowHeight="3600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="8580" windowHeight="3600"/>
   </bookViews>
   <sheets>
     <sheet name="Obama" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Insidious!&lt;e&gt;Mitt Romney&lt;/e&gt;'s Bain Helped Philip Morris Get U.S. High Schoolers &lt;a&gt;Hooked On Cigarettes&lt;/a&gt; http://t.co/nMKuFcUq via @HuffPostPol</t>
   </si>
@@ -33,11 +33,23 @@
   <si>
     <t>&lt;e&gt;Mitt Romney&lt;/e&gt; still doesn't &lt;a&gt;believe&lt;/a&gt; that we &lt;a&gt;have a black president&lt;/a&gt;.</t>
   </si>
+  <si>
+    <t>&lt;e&gt;Barack Obama&lt;/e&gt; still doesn't &lt;a&gt;believe&lt;/a&gt; that we &lt;a&gt;have a black president&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Insidious!&lt;e&gt;Barack Obama&lt;/e&gt;'s Bain Helped Philip Morris Get U.S. High Schoolers &lt;a&gt;Hooked On Cigarettes&lt;/a&gt; http://t.co/nMKuFcUq via @HuffPostPol</t>
+  </si>
+  <si>
+    <t>.@WardBrenda @shortwave8669 @allanbourdius you mean like &lt;e&gt;obama &lt;/e&gt;&lt;a&gt;cheated in primary&lt;/a&gt;?</t>
+  </si>
+  <si>
+    <t>Senior &lt;e&gt;Obama&lt;/e&gt; Advisor Claims &lt;e&gt;Romney&lt;/e&gt; Administration Is Deliberately &lt;a&gt;Misleading Public On Libya&lt;/a&gt;: http://t.co/cpJjGsCF tp #US</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -574,11 +586,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A061A1-26B1-4010-8637-3E3214E2C8FF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -588,7 +600,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -596,7 +608,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -604,7 +616,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -612,7 +624,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -621,11 +633,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>